<commit_message>
AMEND GUOTAI_N DELIVERY DATA TEMPLATE
</commit_message>
<xml_diff>
--- a/src/Presentation/CTM.Win/DataTemplate/Delivery/GuoTai_N.xlsx
+++ b/src/Presentation/CTM.Win/DataTemplate/Delivery/GuoTai_N.xlsx
@@ -14,29 +14,100 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
+  <si>
+    <t>成交日期</t>
+  </si>
+  <si>
+    <t>成交时间</t>
+  </si>
+  <si>
+    <t>证券代码</t>
+  </si>
+  <si>
+    <t>证券名称</t>
+  </si>
+  <si>
+    <t>操作</t>
+  </si>
+  <si>
+    <t>成交数量</t>
+  </si>
+  <si>
+    <t>成交编号</t>
+  </si>
+  <si>
+    <t>成交均价</t>
+  </si>
+  <si>
+    <t>成交金额</t>
+  </si>
+  <si>
+    <t>本次余额</t>
+  </si>
+  <si>
+    <t>股票余额</t>
+  </si>
+  <si>
+    <t>发生金额</t>
+  </si>
+  <si>
+    <t>手续费</t>
+  </si>
+  <si>
+    <t>印花税</t>
+  </si>
+  <si>
+    <t>其他杂费</t>
+  </si>
+  <si>
+    <t>资金余额</t>
+  </si>
+  <si>
+    <t>本次金额</t>
+  </si>
+  <si>
+    <t>合同编号</t>
+  </si>
+  <si>
+    <t>市场名称</t>
+  </si>
+  <si>
+    <t>股东帐户</t>
+  </si>
+  <si>
+    <t>币种</t>
+  </si>
   <si>
     <t>交易类别</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>日内</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>人民币</t>
   </si>
   <si>
     <t>波段</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>目标</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>帝王洁具</t>
+  </si>
+  <si>
+    <t>证券买入</t>
+  </si>
+  <si>
+    <t>深圳Ａ股</t>
+  </si>
+  <si>
+    <t>波段</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,6 +119,13 @@
       <sz val="9"/>
       <name val="宋体"/>
       <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -72,9 +150,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -381,202 +462,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="18" max="18" width="14.5" customWidth="1"/>
+    <col min="1" max="3" width="9" style="1"/>
+    <col min="4" max="4" width="13.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="1"/>
+    <col min="7" max="7" width="12.375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="str">
-        <f>"成交日期"</f>
-        <v>成交日期</v>
-      </c>
-      <c r="B1" s="1" t="str">
-        <f>"业务名称"</f>
-        <v>业务名称</v>
-      </c>
-      <c r="C1" s="1" t="str">
-        <f>"证券代码"</f>
-        <v>证券代码</v>
-      </c>
-      <c r="D1" s="1" t="str">
-        <f>"证券名称"</f>
-        <v>证券名称</v>
-      </c>
-      <c r="E1" s="1" t="str">
-        <f>"成交价格"</f>
-        <v>成交价格</v>
-      </c>
-      <c r="F1" s="1" t="str">
-        <f>"成交数量"</f>
-        <v>成交数量</v>
-      </c>
-      <c r="G1" s="1" t="str">
-        <f>"剩余数量"</f>
-        <v>剩余数量</v>
-      </c>
-      <c r="H1" s="1" t="str">
-        <f>"成交金额"</f>
-        <v>成交金额</v>
-      </c>
-      <c r="I1" s="1" t="str">
-        <f>"清算金额"</f>
-        <v>清算金额</v>
-      </c>
-      <c r="J1" s="1" t="str">
-        <f>"剩余金额"</f>
-        <v>剩余金额</v>
-      </c>
-      <c r="K1" s="1" t="str">
-        <f>"净佣金"</f>
-        <v>净佣金</v>
-      </c>
-      <c r="L1" s="1" t="str">
-        <f>"规费"</f>
-        <v>规费</v>
-      </c>
-      <c r="M1" s="1" t="str">
-        <f>"印花税"</f>
-        <v>印花税</v>
-      </c>
-      <c r="N1" s="1" t="str">
-        <f>"过户费"</f>
-        <v>过户费</v>
-      </c>
-      <c r="O1" s="1" t="str">
-        <f>"结算费"</f>
-        <v>结算费</v>
-      </c>
-      <c r="P1" s="1" t="str">
-        <f>"附加费"</f>
-        <v>附加费</v>
-      </c>
-      <c r="Q1" s="1" t="str">
-        <f>"成交编号"</f>
-        <v>成交编号</v>
-      </c>
-      <c r="R1" s="1" t="str">
-        <f>"股东代码"</f>
-        <v>股东代码</v>
-      </c>
-      <c r="S1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="str">
-        <f t="shared" ref="A2:A4" si="0">"20160729"</f>
-        <v>20160729</v>
-      </c>
-      <c r="B2" s="1" t="str">
-        <f t="shared" ref="B2" si="1">"融资买入"</f>
-        <v>融资买入</v>
-      </c>
-      <c r="C2" s="1" t="str">
-        <f t="shared" ref="C2" si="2">"601336"</f>
-        <v>601336</v>
-      </c>
-      <c r="D2" s="1" t="str">
-        <f t="shared" ref="D2" si="3">"新华保险"</f>
-        <v>新华保险</v>
-      </c>
-      <c r="E2" s="1">
-        <v>39.799999999999997</v>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
+        <v>20170526</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.43089120370370365</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2798</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="F2" s="1">
-        <v>97000</v>
+        <v>5100</v>
       </c>
       <c r="G2" s="1">
-        <v>228600</v>
+        <v>103000004248426</v>
       </c>
       <c r="H2" s="1">
-        <v>3860553</v>
+        <v>37.396999999999998</v>
       </c>
       <c r="I2" s="1">
-        <v>-3861595.35</v>
+        <v>190725</v>
       </c>
       <c r="J2" s="1">
-        <v>409555.31</v>
+        <v>23900</v>
       </c>
       <c r="K2" s="1">
-        <v>699.92</v>
+        <v>23900</v>
       </c>
       <c r="L2" s="1">
-        <v>265.22000000000003</v>
+        <v>-190772.68</v>
       </c>
       <c r="M2" s="1">
-        <v>0</v>
+        <v>47.68</v>
       </c>
       <c r="N2" s="1">
-        <v>77.209999999999994</v>
+        <v>0</v>
       </c>
       <c r="O2" s="1">
         <v>0</v>
       </c>
       <c r="P2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="1" t="str">
-        <f>"1805700502"</f>
-        <v>1805700502</v>
-      </c>
-      <c r="R2" s="1" t="str">
-        <f t="shared" ref="R2" si="4">"E042902565"</f>
-        <v>E042902565</v>
-      </c>
-      <c r="S2" t="s">
-        <v>1</v>
+        <v>112618.45</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>112618.45</v>
+      </c>
+      <c r="R2" s="1">
+        <v>103000004248426</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T2" s="1">
+        <v>181570177</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>20160729</v>
-      </c>
-      <c r="B3" s="1" t="str">
-        <f>"普通卖出"</f>
-        <v>普通卖出</v>
-      </c>
-      <c r="C3" s="1" t="str">
-        <f>"000002"</f>
-        <v>000002</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <f>"万 科Ａ"</f>
-        <v>万 科Ａ</v>
-      </c>
-      <c r="E3" s="1">
-        <v>16.850000000000001</v>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
+        <v>20170526</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.43079861111111112</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2798</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="F3" s="1">
-        <v>207000</v>
+        <v>4100</v>
       </c>
       <c r="G3" s="1">
-        <v>138138</v>
+        <v>103000004241161</v>
       </c>
       <c r="H3" s="1">
-        <v>3487950</v>
+        <v>37.292999999999999</v>
       </c>
       <c r="I3" s="1">
-        <v>3483589.73</v>
+        <v>152900</v>
       </c>
       <c r="J3" s="1">
-        <v>1983628.78</v>
+        <v>18800</v>
       </c>
       <c r="K3" s="1">
-        <v>562.79</v>
+        <v>18800</v>
       </c>
       <c r="L3" s="1">
-        <v>309.2</v>
+        <v>-152938.23000000001</v>
       </c>
       <c r="M3" s="1">
-        <v>3488.28</v>
+        <v>38.229999999999997</v>
       </c>
       <c r="N3" s="1">
         <v>0</v>
@@ -585,63 +661,66 @@
         <v>0</v>
       </c>
       <c r="P3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1" t="str">
-        <f>"F6700159"</f>
-        <v>F6700159</v>
-      </c>
-      <c r="R3" s="1" t="str">
-        <f t="shared" ref="R3:R4" si="5">"0604291857"</f>
-        <v>0604291857</v>
-      </c>
-      <c r="S3" t="s">
-        <v>2</v>
+        <v>303391.13</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>303391.13</v>
+      </c>
+      <c r="R3" s="1">
+        <v>103000004241161</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" s="1">
+        <v>181570177</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>20160729</v>
-      </c>
-      <c r="B4" s="1" t="str">
-        <f t="shared" ref="B4" si="6">"普通买入"</f>
-        <v>普通买入</v>
-      </c>
-      <c r="C4" s="1" t="str">
-        <f>"002798"</f>
-        <v>002798</v>
-      </c>
-      <c r="D4" s="1" t="str">
-        <f>"帝王洁具"</f>
-        <v>帝王洁具</v>
-      </c>
-      <c r="E4" s="1">
-        <v>65.8</v>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
+        <v>20170526</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.43063657407407407</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2798</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="F4" s="1">
-        <v>11300</v>
+        <v>2600</v>
       </c>
       <c r="G4" s="1">
-        <v>70133</v>
+        <v>103000004227691</v>
       </c>
       <c r="H4" s="1">
-        <v>743540</v>
+        <v>37.137</v>
       </c>
       <c r="I4" s="1">
-        <v>-743725.89</v>
+        <v>96555</v>
       </c>
       <c r="J4" s="1">
-        <v>172057</v>
+        <v>14700</v>
       </c>
       <c r="K4" s="1">
-        <v>120.01</v>
+        <v>14700</v>
       </c>
       <c r="L4" s="1">
-        <v>65.88</v>
+        <v>-96579.14</v>
       </c>
       <c r="M4" s="1">
-        <v>0</v>
+        <v>24.14</v>
       </c>
       <c r="N4" s="1">
         <v>0</v>
@@ -650,18 +729,297 @@
         <v>0</v>
       </c>
       <c r="P4" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="1" t="str">
-        <f>"F6700193"</f>
-        <v>F6700193</v>
-      </c>
-      <c r="R4" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>0604291857</v>
-      </c>
-      <c r="S4" t="s">
-        <v>3</v>
+        <v>456329.36</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>456329.36</v>
+      </c>
+      <c r="R4" s="1">
+        <v>103000004227691</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T4" s="1">
+        <v>181570177</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A5" s="1">
+        <v>20170526</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.43056712962962962</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2798</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="1">
+        <v>5100</v>
+      </c>
+      <c r="G5" s="1">
+        <v>103000004222751</v>
+      </c>
+      <c r="H5" s="1">
+        <v>37.119999999999997</v>
+      </c>
+      <c r="I5" s="1">
+        <v>189312</v>
+      </c>
+      <c r="J5" s="1">
+        <v>12100</v>
+      </c>
+      <c r="K5" s="1">
+        <v>12100</v>
+      </c>
+      <c r="L5" s="1">
+        <v>-189359.33</v>
+      </c>
+      <c r="M5" s="1">
+        <v>47.33</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>552908.5</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>552908.5</v>
+      </c>
+      <c r="R5" s="1">
+        <v>103000004222751</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T5" s="1">
+        <v>181570177</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A6" s="1">
+        <v>20170526</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.43053240740740745</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2798</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3500</v>
+      </c>
+      <c r="G6" s="1">
+        <v>103000004221147</v>
+      </c>
+      <c r="H6" s="1">
+        <v>37.11</v>
+      </c>
+      <c r="I6" s="1">
+        <v>129885</v>
+      </c>
+      <c r="J6" s="1">
+        <v>7000</v>
+      </c>
+      <c r="K6" s="1">
+        <v>7000</v>
+      </c>
+      <c r="L6" s="1">
+        <v>-129917.47</v>
+      </c>
+      <c r="M6" s="1">
+        <v>32.47</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1">
+        <v>742267.83</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>742267.83</v>
+      </c>
+      <c r="R6" s="1">
+        <v>103000004221147</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T6" s="1">
+        <v>181570177</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
+        <v>20170526</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.43049768518518516</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2798</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2100</v>
+      </c>
+      <c r="G7" s="1">
+        <v>103000004216460</v>
+      </c>
+      <c r="H7" s="1">
+        <v>37.11</v>
+      </c>
+      <c r="I7" s="1">
+        <v>77931</v>
+      </c>
+      <c r="J7" s="1">
+        <v>3500</v>
+      </c>
+      <c r="K7" s="1">
+        <v>3500</v>
+      </c>
+      <c r="L7" s="1">
+        <v>-77950.48</v>
+      </c>
+      <c r="M7" s="1">
+        <v>19.48</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <v>872185.3</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>872185.3</v>
+      </c>
+      <c r="R7" s="1">
+        <v>103000004216460</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T7" s="1">
+        <v>181570177</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A8" s="1">
+        <v>20170526</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.43045138888888884</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2798</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1400</v>
+      </c>
+      <c r="G8" s="1">
+        <v>103000004213069</v>
+      </c>
+      <c r="H8" s="1">
+        <v>37.11</v>
+      </c>
+      <c r="I8" s="1">
+        <v>51954</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1400</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1400</v>
+      </c>
+      <c r="L8" s="1">
+        <v>-51966.99</v>
+      </c>
+      <c r="M8" s="1">
+        <v>12.99</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1">
+        <v>950135.78</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>950135.78</v>
+      </c>
+      <c r="R8" s="1">
+        <v>103000004213069</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T8" s="1">
+        <v>181570177</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>